<commit_message>
Updated Plotting Scripts 06/18
</commit_message>
<xml_diff>
--- a/Safe_Results/SA_Capacity_Costs/SA_Capacity_Costs_HPHB.xlsx
+++ b/Safe_Results/SA_Capacity_Costs/SA_Capacity_Costs_HPHB.xlsx
@@ -521,46 +521,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.8584</v>
+        <v>5.45195</v>
       </c>
       <c r="C2" t="n">
-        <v>6.04675</v>
+        <v>5.89945</v>
       </c>
       <c r="D2" t="n">
-        <v>37.04525</v>
+        <v>37.50169999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08230000000000001</v>
+        <v>0.17115</v>
       </c>
       <c r="F2" t="n">
-        <v>2290.62735</v>
+        <v>2219.401700000001</v>
       </c>
       <c r="G2" t="n">
-        <v>2062.7902</v>
+        <v>2014.1057</v>
       </c>
       <c r="H2" t="n">
-        <v>227.8371</v>
+        <v>205.29605</v>
       </c>
       <c r="I2" t="n">
-        <v>227.8371</v>
+        <v>205.29605</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2839.3604</v>
+        <v>2798.105</v>
       </c>
       <c r="L2" t="n">
-        <v>2062.796</v>
+        <v>2014.125</v>
       </c>
       <c r="M2" t="n">
-        <v>776.5644</v>
+        <v>783.98</v>
       </c>
       <c r="N2" t="n">
-        <v>372.4055999999999</v>
+        <v>345.6012</v>
       </c>
       <c r="O2" t="n">
-        <v>404.1588</v>
+        <v>438.3792</v>
       </c>
     </row>
     <row r="3">
@@ -570,46 +570,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.134</v>
+        <v>5.789</v>
       </c>
       <c r="C3" t="n">
-        <v>9.683</v>
+        <v>9.571999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>27.468</v>
+        <v>28.079</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2400.139</v>
+        <v>2327.595</v>
       </c>
       <c r="G3" t="n">
-        <v>2162.645</v>
+        <v>2122.899</v>
       </c>
       <c r="H3" t="n">
-        <v>237.494</v>
+        <v>204.696</v>
       </c>
       <c r="I3" t="n">
-        <v>222.258</v>
+        <v>193.677</v>
       </c>
       <c r="J3" t="n">
-        <v>15.236</v>
+        <v>11.019</v>
       </c>
       <c r="K3" t="n">
-        <v>2558.546</v>
+        <v>2476.9342</v>
       </c>
       <c r="L3" t="n">
-        <v>2162.609</v>
+        <v>2122.95</v>
       </c>
       <c r="M3" t="n">
-        <v>395.937</v>
+        <v>353.9842</v>
       </c>
       <c r="N3" t="n">
-        <v>341.1596</v>
+        <v>308.7674</v>
       </c>
       <c r="O3" t="n">
-        <v>54.7774</v>
+        <v>45.2168</v>
       </c>
     </row>
     <row r="4">
@@ -619,46 +619,46 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.022</v>
+        <v>6.746</v>
       </c>
       <c r="C4" t="n">
-        <v>8.914</v>
+        <v>8.249000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>36.723</v>
+        <v>41.042</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2589.978</v>
+        <v>2510.203</v>
       </c>
       <c r="G4" t="n">
-        <v>2305.23</v>
+        <v>2280.003</v>
       </c>
       <c r="H4" t="n">
-        <v>284.748</v>
+        <v>230.2</v>
       </c>
       <c r="I4" t="n">
-        <v>284.748</v>
+        <v>64.40900000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>165.791</v>
       </c>
       <c r="K4" t="n">
-        <v>2542.9758</v>
+        <v>2467.796</v>
       </c>
       <c r="L4" t="n">
-        <v>2305.23</v>
+        <v>2280.003</v>
       </c>
       <c r="M4" t="n">
-        <v>237.7458</v>
+        <v>187.793</v>
       </c>
       <c r="N4" t="n">
-        <v>217.774</v>
+        <v>176.6258</v>
       </c>
       <c r="O4" t="n">
-        <v>19.9718</v>
+        <v>11.1674</v>
       </c>
     </row>
   </sheetData>
@@ -764,43 +764,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.9663</v>
+        <v>5.591900000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>6.7075</v>
+        <v>6.396350000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>36.2501</v>
+        <v>36.86314999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08020000000000001</v>
+        <v>0.1292</v>
       </c>
       <c r="F2" t="n">
-        <v>2324.3994</v>
+        <v>2253.7439</v>
       </c>
       <c r="G2" t="n">
-        <v>2094.81395</v>
+        <v>2044.3985</v>
       </c>
       <c r="H2" t="n">
-        <v>229.5853999999999</v>
+        <v>209.34555</v>
       </c>
       <c r="I2" t="n">
-        <v>229.5853999999999</v>
+        <v>209.34555</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2365.7068</v>
+        <v>2285.459</v>
       </c>
       <c r="L2" t="n">
-        <v>2094.82</v>
+        <v>2044.411</v>
       </c>
       <c r="M2" t="n">
-        <v>270.8868</v>
+        <v>241.048</v>
       </c>
       <c r="N2" t="n">
-        <v>270.8868</v>
+        <v>241.048</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -813,43 +813,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.438</v>
+        <v>5.963</v>
       </c>
       <c r="C3" t="n">
-        <v>9.507</v>
+        <v>9.461</v>
       </c>
       <c r="D3" t="n">
-        <v>28.465</v>
+        <v>28.427</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2432.563</v>
+        <v>2359.512</v>
       </c>
       <c r="G3" t="n">
-        <v>2198.519</v>
+        <v>2141.396</v>
       </c>
       <c r="H3" t="n">
-        <v>234.044</v>
+        <v>218.116</v>
       </c>
       <c r="I3" t="n">
-        <v>213.691</v>
+        <v>201.182</v>
       </c>
       <c r="J3" t="n">
-        <v>20.353</v>
+        <v>16.934</v>
       </c>
       <c r="K3" t="n">
-        <v>2426.2362</v>
+        <v>2347.4208</v>
       </c>
       <c r="L3" t="n">
-        <v>2198.507</v>
+        <v>2141.429</v>
       </c>
       <c r="M3" t="n">
-        <v>227.7292</v>
+        <v>205.9918</v>
       </c>
       <c r="N3" t="n">
-        <v>227.7292</v>
+        <v>205.9918</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -862,43 +862,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.025</v>
+        <v>6.7</v>
       </c>
       <c r="C4" t="n">
-        <v>8.618</v>
+        <v>8.093999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>47.282</v>
+        <v>47.574</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2674.647</v>
+        <v>2580.234</v>
       </c>
       <c r="G4" t="n">
-        <v>2373.396</v>
+        <v>2317.715</v>
       </c>
       <c r="H4" t="n">
-        <v>301.251</v>
+        <v>262.519</v>
       </c>
       <c r="I4" t="n">
-        <v>158.192</v>
+        <v>54.052</v>
       </c>
       <c r="J4" t="n">
-        <v>143.058</v>
+        <v>208.467</v>
       </c>
       <c r="K4" t="n">
-        <v>2470.723800000001</v>
+        <v>2395.058</v>
       </c>
       <c r="L4" t="n">
-        <v>2373.396</v>
+        <v>2317.715</v>
       </c>
       <c r="M4" t="n">
-        <v>97.3278</v>
+        <v>77.343</v>
       </c>
       <c r="N4" t="n">
-        <v>97.3278</v>
+        <v>77.343</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -1007,46 +1007,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.8099</v>
+        <v>5.43975</v>
       </c>
       <c r="C2" t="n">
-        <v>6.332949999999999</v>
+        <v>6.10355</v>
       </c>
       <c r="D2" t="n">
-        <v>36.52495</v>
+        <v>37.0707</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08230000000000001</v>
+        <v>0.17115</v>
       </c>
       <c r="F2" t="n">
-        <v>2294.0657</v>
+        <v>2222.8903</v>
       </c>
       <c r="G2" t="n">
-        <v>2064.3211</v>
+        <v>2017.33845</v>
       </c>
       <c r="H2" t="n">
-        <v>229.74445</v>
+        <v>205.55185</v>
       </c>
       <c r="I2" t="n">
-        <v>229.74445</v>
+        <v>205.55185</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2869.2772</v>
+        <v>2804.228</v>
       </c>
       <c r="L2" t="n">
-        <v>2064.323</v>
+        <v>2017.357</v>
       </c>
       <c r="M2" t="n">
-        <v>804.9542</v>
+        <v>786.8710000000001</v>
       </c>
       <c r="N2" t="n">
-        <v>392.7458</v>
+        <v>359.913</v>
       </c>
       <c r="O2" t="n">
-        <v>412.2084</v>
+        <v>426.9582</v>
       </c>
     </row>
     <row r="3">
@@ -1056,46 +1056,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.931</v>
+        <v>5.483</v>
       </c>
       <c r="C3" t="n">
-        <v>7.777</v>
+        <v>7.719</v>
       </c>
       <c r="D3" t="n">
-        <v>32.754</v>
+        <v>32.87</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2390.068</v>
+        <v>2320.004</v>
       </c>
       <c r="G3" t="n">
-        <v>2105.207</v>
+        <v>2051.97</v>
       </c>
       <c r="H3" t="n">
-        <v>284.86</v>
+        <v>268.033</v>
       </c>
       <c r="I3" t="n">
-        <v>236.824</v>
+        <v>220.571</v>
       </c>
       <c r="J3" t="n">
-        <v>48.037</v>
+        <v>47.462</v>
       </c>
       <c r="K3" t="n">
-        <v>2700.518799999999</v>
+        <v>2618.863</v>
       </c>
       <c r="L3" t="n">
-        <v>2105.182</v>
+        <v>2051.924</v>
       </c>
       <c r="M3" t="n">
-        <v>595.3368</v>
+        <v>566.939</v>
       </c>
       <c r="N3" t="n">
-        <v>375.419</v>
+        <v>353.6808</v>
       </c>
       <c r="O3" t="n">
-        <v>219.9178</v>
+        <v>213.2584</v>
       </c>
     </row>
     <row r="4">
@@ -1105,46 +1105,46 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.817</v>
+        <v>6.231</v>
       </c>
       <c r="C4" t="n">
-        <v>8.097</v>
+        <v>8.112</v>
       </c>
       <c r="D4" t="n">
-        <v>46.17</v>
+        <v>43.556</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2660.138</v>
+        <v>2573.291</v>
       </c>
       <c r="G4" t="n">
-        <v>2320.845</v>
+        <v>2233.933</v>
       </c>
       <c r="H4" t="n">
-        <v>339.293</v>
+        <v>339.358</v>
       </c>
       <c r="I4" t="n">
-        <v>114.329</v>
+        <v>119.435</v>
       </c>
       <c r="J4" t="n">
-        <v>224.964</v>
+        <v>219.923</v>
       </c>
       <c r="K4" t="n">
-        <v>2576.5094</v>
+        <v>2490.067</v>
       </c>
       <c r="L4" t="n">
-        <v>2320.845</v>
+        <v>2233.933</v>
       </c>
       <c r="M4" t="n">
-        <v>255.6644</v>
+        <v>256.134</v>
       </c>
       <c r="N4" t="n">
-        <v>185.8148</v>
+        <v>190.343</v>
       </c>
       <c r="O4" t="n">
-        <v>69.8496</v>
+        <v>65.791</v>
       </c>
     </row>
   </sheetData>
@@ -1250,46 +1250,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.0771</v>
+        <v>5.734050000000002</v>
       </c>
       <c r="C2" t="n">
-        <v>6.4457</v>
+        <v>6.146849999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>38.5994</v>
+        <v>39.35619999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.003700000000000001</v>
+        <v>0.04355</v>
       </c>
       <c r="F2" t="n">
-        <v>2367.3184</v>
+        <v>2295.672100000001</v>
       </c>
       <c r="G2" t="n">
-        <v>2114.6003</v>
+        <v>2069.291249999999</v>
       </c>
       <c r="H2" t="n">
-        <v>252.71795</v>
+        <v>226.3809</v>
       </c>
       <c r="I2" t="n">
-        <v>252.71795</v>
+        <v>226.3809</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2258.917</v>
+        <v>2185.4816</v>
       </c>
       <c r="L2" t="n">
-        <v>2114.603</v>
+        <v>2069.311</v>
       </c>
       <c r="M2" t="n">
-        <v>144.314</v>
+        <v>116.1706</v>
       </c>
       <c r="N2" t="n">
-        <v>96.1254</v>
+        <v>80.70360000000001</v>
       </c>
       <c r="O2" t="n">
-        <v>48.1886</v>
+        <v>35.467</v>
       </c>
     </row>
     <row r="3">
@@ -1299,43 +1299,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.604</v>
+        <v>6.113</v>
       </c>
       <c r="C3" t="n">
-        <v>9.411</v>
+        <v>9.366</v>
       </c>
       <c r="D3" t="n">
-        <v>29.692</v>
+        <v>29.606</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2466.778</v>
+        <v>2390.136</v>
       </c>
       <c r="G3" t="n">
-        <v>2223.196</v>
+        <v>2164.023</v>
       </c>
       <c r="H3" t="n">
-        <v>243.582</v>
+        <v>226.112</v>
       </c>
       <c r="I3" t="n">
-        <v>227.899</v>
+        <v>213.845</v>
       </c>
       <c r="J3" t="n">
-        <v>15.683</v>
+        <v>12.267</v>
       </c>
       <c r="K3" t="n">
-        <v>2296.4916</v>
+        <v>2231.9788</v>
       </c>
       <c r="L3" t="n">
-        <v>2223.236</v>
+        <v>2163.984</v>
       </c>
       <c r="M3" t="n">
-        <v>73.25559999999999</v>
+        <v>67.9948</v>
       </c>
       <c r="N3" t="n">
-        <v>73.25559999999999</v>
+        <v>67.9948</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -1348,43 +1348,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.025</v>
+        <v>6.7</v>
       </c>
       <c r="C4" t="n">
-        <v>8.618</v>
+        <v>8.093999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>47.282</v>
+        <v>47.574</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2674.647</v>
+        <v>2580.234</v>
       </c>
       <c r="G4" t="n">
-        <v>2373.396</v>
+        <v>2317.715</v>
       </c>
       <c r="H4" t="n">
-        <v>301.251</v>
+        <v>262.519</v>
       </c>
       <c r="I4" t="n">
-        <v>158.192</v>
+        <v>54.052</v>
       </c>
       <c r="J4" t="n">
-        <v>143.058</v>
+        <v>208.467</v>
       </c>
       <c r="K4" t="n">
-        <v>2390.0244</v>
+        <v>2328.9178</v>
       </c>
       <c r="L4" t="n">
-        <v>2373.396</v>
+        <v>2317.715</v>
       </c>
       <c r="M4" t="n">
-        <v>16.6284</v>
+        <v>11.2028</v>
       </c>
       <c r="N4" t="n">
-        <v>16.6284</v>
+        <v>11.2028</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -1493,46 +1493,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.0077</v>
+        <v>5.656750000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>6.2403</v>
+        <v>5.934599999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>38.8293</v>
+        <v>39.77945</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08070000000000001</v>
+        <v>0.16955</v>
       </c>
       <c r="F2" t="n">
-        <v>2341.10255</v>
+        <v>2266.771</v>
       </c>
       <c r="G2" t="n">
-        <v>2100.92505</v>
+        <v>2056.2701</v>
       </c>
       <c r="H2" t="n">
-        <v>240.1773000000001</v>
+        <v>210.50085</v>
       </c>
       <c r="I2" t="n">
-        <v>240.1773000000001</v>
+        <v>210.50085</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2441.6388</v>
+        <v>2393.0558</v>
       </c>
       <c r="L2" t="n">
-        <v>2100.938</v>
+        <v>2056.285</v>
       </c>
       <c r="M2" t="n">
-        <v>340.7008</v>
+        <v>336.7708</v>
       </c>
       <c r="N2" t="n">
-        <v>171.998</v>
+        <v>152.2866</v>
       </c>
       <c r="O2" t="n">
-        <v>168.703</v>
+        <v>184.4844</v>
       </c>
     </row>
     <row r="3">
@@ -1542,46 +1542,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.575</v>
+        <v>6.099</v>
       </c>
       <c r="C3" t="n">
-        <v>7.969</v>
+        <v>7.875</v>
       </c>
       <c r="D3" t="n">
-        <v>34.013</v>
+        <v>33.748</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2447.077</v>
+        <v>2371.432</v>
       </c>
       <c r="G3" t="n">
-        <v>2196.681</v>
+        <v>2135.853</v>
       </c>
       <c r="H3" t="n">
-        <v>250.396</v>
+        <v>235.579</v>
       </c>
       <c r="I3" t="n">
-        <v>211.053</v>
+        <v>199.385</v>
       </c>
       <c r="J3" t="n">
-        <v>39.343</v>
+        <v>36.195</v>
       </c>
       <c r="K3" t="n">
-        <v>2400.2378</v>
+        <v>2332.4364</v>
       </c>
       <c r="L3" t="n">
-        <v>2196.634</v>
+        <v>2135.884</v>
       </c>
       <c r="M3" t="n">
-        <v>203.6038</v>
+        <v>196.5524</v>
       </c>
       <c r="N3" t="n">
-        <v>135.9896</v>
+        <v>126.9988</v>
       </c>
       <c r="O3" t="n">
-        <v>67.61420000000001</v>
+        <v>69.5534</v>
       </c>
     </row>
     <row r="4">
@@ -1591,46 +1591,46 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.025</v>
+        <v>7.162</v>
       </c>
       <c r="C4" t="n">
-        <v>8.618</v>
+        <v>7.283</v>
       </c>
       <c r="D4" t="n">
-        <v>47.282</v>
+        <v>49.794</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2674.647</v>
+        <v>2576.937</v>
       </c>
       <c r="G4" t="n">
-        <v>2373.396</v>
+        <v>2356.575</v>
       </c>
       <c r="H4" t="n">
-        <v>301.251</v>
+        <v>220.362</v>
       </c>
       <c r="I4" t="n">
-        <v>158.192</v>
+        <v>121.688</v>
       </c>
       <c r="J4" t="n">
-        <v>143.058</v>
+        <v>98.675</v>
       </c>
       <c r="K4" t="n">
-        <v>2464.626</v>
+        <v>2467.0234</v>
       </c>
       <c r="L4" t="n">
-        <v>2373.396</v>
+        <v>2356.575</v>
       </c>
       <c r="M4" t="n">
-        <v>91.22999999999999</v>
+        <v>110.4484</v>
       </c>
       <c r="N4" t="n">
-        <v>65.83019999999999</v>
+        <v>44.6264</v>
       </c>
       <c r="O4" t="n">
-        <v>25.3998</v>
+        <v>65.8222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>